<commit_message>
Update vendor mapping functionality and UI improvements
🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/vendor_selections.xlsx
+++ b/data/vendor_selections.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>client_id</t>
   </si>
@@ -40,22 +40,73 @@
     <t>LTRADC.ahm.lambdacro.com</t>
   </si>
   <si>
+    <t>PV_RPT_DB.ahm.lambdacro.com</t>
+  </si>
+  <si>
+    <t>AHM_PRD_NAS</t>
+  </si>
+  <si>
+    <t>MEH_PRD_NAS</t>
+  </si>
+  <si>
+    <t>HOST-3.123.68.65</t>
+  </si>
+  <si>
+    <t>AHM_VCenter</t>
+  </si>
+  <si>
+    <t>LTRPDC.ahm.lambdacro.com</t>
+  </si>
+  <si>
     <t>TrendMicro</t>
   </si>
   <si>
     <t>Microsoft</t>
   </si>
   <si>
+    <t>Synology</t>
+  </si>
+  <si>
+    <t>Fortinet</t>
+  </si>
+  <si>
+    <t>VMware</t>
+  </si>
+  <si>
     <t>Vision One</t>
   </si>
   <si>
     <t>Windows</t>
   </si>
   <si>
+    <t>Windows Server 2022</t>
+  </si>
+  <si>
+    <t>NAS</t>
+  </si>
+  <si>
+    <t>FortiWeb Cloud</t>
+  </si>
+  <si>
+    <t>vCenter</t>
+  </si>
+  <si>
     <t>2025-12-25 16:45:22</t>
   </si>
   <si>
     <t>2025-12-25 16:47:38</t>
+  </si>
+  <si>
+    <t>2025-12-25 17:25:46</t>
+  </si>
+  <si>
+    <t>2025-12-25 17:25:49</t>
+  </si>
+  <si>
+    <t>2025-12-25 17:26:41</t>
+  </si>
+  <si>
+    <t>2025-12-25 17:26:53</t>
   </si>
 </sst>
 </file>
@@ -413,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,16 +498,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -467,16 +518,136 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working before adding escalted incindets
🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/vendor_selections.xlsx
+++ b/data/vendor_selections.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>client_id</t>
   </si>
@@ -34,79 +34,157 @@
     <t>updated_at</t>
   </si>
   <si>
+    <t>CDMO_PRD_AHM</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>MEH_PRD_NAS</t>
+  </si>
+  <si>
+    <t>LAMFILE_NAS</t>
+  </si>
+  <si>
+    <t>ARCHIVAL_AHM_NAS</t>
+  </si>
+  <si>
+    <t>MEHLAMFILE_NAS</t>
+  </si>
+  <si>
+    <t>Lambda-Changodar-60F</t>
+  </si>
+  <si>
+    <t>Fortigate_Firewall_Ahm_OT</t>
+  </si>
+  <si>
+    <t>Lambda_MEH_FW-100F</t>
+  </si>
+  <si>
+    <t>AHM_PRD_NAS</t>
+  </si>
+  <si>
+    <t>HOST-3.123.68.65</t>
+  </si>
+  <si>
+    <t>LTRADC.ahm.lambdacro.com</t>
+  </si>
+  <si>
+    <t>LTRPDC.ahm.lambdacro.com</t>
+  </si>
+  <si>
     <t>Lambda.coll</t>
   </si>
   <si>
-    <t>LTRADC.ahm.lambdacro.com</t>
-  </si>
-  <si>
     <t>PV_RPT_DB.ahm.lambdacro.com</t>
   </si>
   <si>
-    <t>AHM_PRD_NAS</t>
-  </si>
-  <si>
-    <t>MEH_PRD_NAS</t>
-  </si>
-  <si>
-    <t>HOST-3.123.68.65</t>
+    <t>HOST-192.168.22.98</t>
+  </si>
+  <si>
+    <t>BIZNET7.ahm.lambdacro.com</t>
   </si>
   <si>
     <t>AHM_VCenter</t>
   </si>
   <si>
-    <t>LTRPDC.ahm.lambdacro.com</t>
-  </si>
-  <si>
-    <t>TrendMicro</t>
+    <t>Lambda_Primary_Firewall-200F</t>
+  </si>
+  <si>
+    <t>HOST-192.168.22.98,Lambda.coll</t>
+  </si>
+  <si>
+    <t>Synology</t>
+  </si>
+  <si>
+    <t>Fortinet</t>
   </si>
   <si>
     <t>Microsoft</t>
   </si>
   <si>
-    <t>Synology</t>
-  </si>
-  <si>
-    <t>Fortinet</t>
+    <t>ManageEngine</t>
   </si>
   <si>
     <t>VMware</t>
   </si>
   <si>
-    <t>Vision One</t>
+    <t>NAS</t>
+  </si>
+  <si>
+    <t>FortiSIEM</t>
+  </si>
+  <si>
+    <t>Fortigate</t>
+  </si>
+  <si>
+    <t>FortiWeb Cloud</t>
   </si>
   <si>
     <t>Windows</t>
   </si>
   <si>
+    <t>ADAuditPlus</t>
+  </si>
+  <si>
     <t>Windows Server 2022</t>
   </si>
   <si>
-    <t>NAS</t>
-  </si>
-  <si>
-    <t>FortiWeb Cloud</t>
-  </si>
-  <si>
     <t>vCenter</t>
   </si>
   <si>
-    <t>2025-12-25 16:45:22</t>
-  </si>
-  <si>
-    <t>2025-12-25 16:47:38</t>
-  </si>
-  <si>
-    <t>2025-12-25 17:25:46</t>
-  </si>
-  <si>
-    <t>2025-12-25 17:25:49</t>
-  </si>
-  <si>
-    <t>2025-12-25 17:26:41</t>
-  </si>
-  <si>
-    <t>2025-12-25 17:26:53</t>
+    <t>2025-12-25 23:00:50</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:00:52</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:00:53</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:00:56</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:00:57</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:00:59</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:05:18</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:05:22</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:07:47</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:07:52</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:06</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:26</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:29</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:42</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:53</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:09:46</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:32</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:08:23</t>
   </si>
 </sst>
 </file>
@@ -464,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,16 +576,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -518,16 +596,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -538,16 +616,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -558,16 +636,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -578,16 +656,16 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -598,16 +676,16 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -618,16 +696,16 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -638,16 +716,256 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
-        <v>30</v>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working after adding true incident
🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/vendor_selections.xlsx
+++ b/data/vendor_selections.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>client_id</t>
   </si>
@@ -184,7 +184,10 @@
     <t>2025-12-25 23:08:32</t>
   </si>
   <si>
-    <t>2025-12-25 23:08:23</t>
+    <t>2025-12-25 23:25:54</t>
+  </si>
+  <si>
+    <t>2025-12-25 23:25:57</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
         <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -765,7 +768,7 @@
         <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -785,7 +788,7 @@
         <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -865,7 +868,7 @@
         <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6">

</xml_diff>

<commit_message>
vendor filter and rule vendor mapping working separately fine
🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/vendor_selections.xlsx
+++ b/data/vendor_selections.xlsx
@@ -184,10 +184,10 @@
     <t>2025-12-25 23:08:32</t>
   </si>
   <si>
-    <t>2025-12-25 23:25:54</t>
-  </si>
-  <si>
-    <t>2025-12-25 23:25:57</t>
+    <t>2025-12-26 00:03:23</t>
+  </si>
+  <si>
+    <t>2025-12-26 00:03:26</t>
   </si>
 </sst>
 </file>

</xml_diff>